<commit_message>
JDBC _02_Soru_2  JDBC Parent
</commit_message>
<xml_diff>
--- a/src/test/java/ApachePOI/resource/ApacheExcel2 (1).xlsx
+++ b/src/test/java/ApachePOI/resource/ApacheExcel2 (1).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechnoStudy\IdeaProjects\Cucumber6\src\test\java\ApachePOI\resource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\muham\IdeaProjects\Cucumber7Ben\src\test\java\ApachePOI\resource\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{730F09CE-D368-4CE6-BC73-7DDDA86FC945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="17280" windowHeight="8970" activeTab="1"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="16199" windowHeight="9307" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Lion</t>
   </si>
@@ -63,58 +64,55 @@
     <t>bes</t>
   </si>
   <si>
-    <t>ulis1111</t>
-  </si>
-  <si>
-    <t>ulis1122</t>
-  </si>
-  <si>
-    <t>ulis1133</t>
-  </si>
-  <si>
-    <t>ulis1144</t>
-  </si>
-  <si>
-    <t>ulis1154</t>
-  </si>
-  <si>
-    <t>ulis1164</t>
-  </si>
-  <si>
-    <t>ulis1174</t>
-  </si>
-  <si>
-    <t>ulis1184</t>
-  </si>
-  <si>
-    <t>ubs13</t>
-  </si>
-  <si>
-    <t>ubs141</t>
-  </si>
-  <si>
-    <t>ubs152</t>
-  </si>
-  <si>
-    <t>ubs162</t>
-  </si>
-  <si>
-    <t>ubs172</t>
-  </si>
-  <si>
-    <t>ubs182</t>
-  </si>
-  <si>
-    <t>ubs192</t>
-  </si>
-  <si>
-    <t>ubs202</t>
+    <t>unbs3475</t>
+  </si>
+  <si>
+    <t>unbs1572</t>
+  </si>
+  <si>
+    <t>unbs1672</t>
+  </si>
+  <si>
+    <t>unbs1772</t>
+  </si>
+  <si>
+    <t>unbs1872</t>
+  </si>
+  <si>
+    <t>unbs1972</t>
+  </si>
+  <si>
+    <t>unbs2072</t>
+  </si>
+  <si>
+    <t>ulims1236</t>
+  </si>
+  <si>
+    <t>ulims1326</t>
+  </si>
+  <si>
+    <t>ulims1446</t>
+  </si>
+  <si>
+    <t>ulims1546</t>
+  </si>
+  <si>
+    <t>ulims1646</t>
+  </si>
+  <si>
+    <t>ulims1746</t>
+  </si>
+  <si>
+    <t>ulims1846</t>
+  </si>
+  <si>
+    <t>unbs2735</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -149,7 +147,7 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -426,16 +424,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -443,7 +441,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -457,7 +455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -465,7 +463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -473,7 +471,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -481,7 +479,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -489,7 +487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -497,7 +495,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -509,164 +507,164 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.06640625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="20.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>9</v>

</xml_diff>